<commit_message>
Update giordano tests, all tests passing
</commit_message>
<xml_diff>
--- a/tests/BatchTest.xlsx
+++ b/tests/BatchTest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/Published Papers/2021_VESIcal/__TheCode/VESIcal_master/VESIcal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/Published Papers/2021_VESIcal/__TheCode/VESIcal_master/VESIcal/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A90FD77-DC01-284C-8F15-BC9663A57AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54F5357-7821-104B-A8F2-067CE5EAA68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D5D8394A-7272-CB4F-A3ED-C86444CC2A22}"/>
+    <workbookView xWindow="6020" yWindow="3620" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D5D8394A-7272-CB4F-A3ED-C86444CC2A22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Label</t>
   </si>
@@ -83,16 +83,10 @@
     <t>test_samp</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>F2O</t>
   </si>
   <si>
     <t>giordano_spreadsheet_default_comp</t>
-  </si>
-  <si>
-    <t>test_w_F</t>
   </si>
 </sst>
 </file>
@@ -547,15 +541,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7889A671-981D-F04B-A273-6F211412B587}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,11 +595,8 @@
       <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -651,13 +642,10 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>62.4</v>
@@ -699,60 +687,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>47.95</v>
-      </c>
-      <c r="C4">
-        <v>1.67</v>
-      </c>
-      <c r="D4">
-        <v>17.32</v>
-      </c>
-      <c r="E4">
-        <v>10.24</v>
-      </c>
-      <c r="F4">
-        <v>0.1</v>
-      </c>
-      <c r="G4">
-        <v>5.76</v>
-      </c>
-      <c r="H4">
-        <v>10.93</v>
-      </c>
-      <c r="I4">
-        <v>3.45</v>
-      </c>
-      <c r="J4">
-        <v>1.99</v>
-      </c>
-      <c r="K4">
-        <v>0.51</v>
-      </c>
-      <c r="L4">
-        <v>0.1</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>0.1</v>
-      </c>
-      <c r="O4">
-        <v>0.5</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>